<commit_message>
Manual testing. Almost all tables
</commit_message>
<xml_diff>
--- a/кейсы.xlsx
+++ b/кейсы.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Приоритет</t>
   </si>
@@ -50,28 +50,67 @@
     <t>Шаг 4</t>
   </si>
   <si>
-    <t>RDM может изменить свой пароль</t>
-  </si>
-  <si>
     <t>Войти в систему под логином RDM</t>
   </si>
   <si>
     <t>Перейти на вкладку "RDM"</t>
   </si>
   <si>
-    <t>Настранице "RDM" рядом с выбранным RDM нажать кнопку "Edit"</t>
-  </si>
-  <si>
-    <t>Пароль RDM изменен и отображается в таблице только для администратора</t>
-  </si>
-  <si>
-    <t>В появившей форме "Edit RDM" все поля не доступны, кроме поля с паролем</t>
-  </si>
-  <si>
-    <t>Изменить поле с паролем и нажать кнопку "Update RDM"</t>
-  </si>
-  <si>
     <t>Шаг 5</t>
+  </si>
+  <si>
+    <t>Совершить выход из приложения с главной страницы при нажатии на кнопку "Logout"</t>
+  </si>
+  <si>
+    <t>Шаг 6</t>
+  </si>
+  <si>
+    <t>Шаг 7</t>
+  </si>
+  <si>
+    <t>Перейти на вкладку "Persons"</t>
+  </si>
+  <si>
+    <t>Совершить выход с текущей вкладки при нажатии на кнопку "Logout"</t>
+  </si>
+  <si>
+    <t>Повторить шаги 3, 4</t>
+  </si>
+  <si>
+    <t>Шаг 8</t>
+  </si>
+  <si>
+    <t>Шаг 9</t>
+  </si>
+  <si>
+    <t>Перейти на вкладку "Requisition"</t>
+  </si>
+  <si>
+    <t>Повторить шаги 6,7</t>
+  </si>
+  <si>
+    <t>Перейти на вкладку "Analysis"</t>
+  </si>
+  <si>
+    <t>Шаг 10</t>
+  </si>
+  <si>
+    <t>Шаг 11</t>
+  </si>
+  <si>
+    <t>Шаг 12</t>
+  </si>
+  <si>
+    <t>Шаг 13</t>
+  </si>
+  <si>
+    <t>RDM может выйти из системы с любой вкладки</t>
+  </si>
+  <si>
+    <t>RDM перешел на стратовую страницу приложения</t>
+  </si>
+  <si>
+    <t>RDM смог выйти из приложения с каждой из вкладок. После выхода он попадает на стартовую страницу приложения</t>
   </si>
 </sst>
 </file>
@@ -123,11 +162,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -447,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E2" sqref="E2:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,83 +505,172 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="4"/>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="3" t="s">
+      <c r="E2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="2" t="s">
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="6"/>
+      <c r="E14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="E2:E14"/>
+    <mergeCell ref="B2:B14"/>
+    <mergeCell ref="A2:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>